<commit_message>
Call center and BE updated
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/CC_CallCenterData.xlsx
+++ b/src/test/resources/testData/CC_CallCenterData.xlsx
@@ -12,7 +12,8 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
   </bookViews>
   <sheets>
-    <sheet name="NormalSingleRoomBookingData" sheetId="1" r:id="rId1"/>
+    <sheet name="NormalSingleRoomBookingData" sheetId="3" r:id="rId1"/>
+    <sheet name="ModifyBookingConfirmationPage" sheetId="4" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="68">
   <si>
     <t>RoomAvailable</t>
   </si>
@@ -116,9 +117,6 @@
     <t>RoomNameModify</t>
   </si>
   <si>
-    <t>Standard room</t>
-  </si>
-  <si>
     <t>CCUser</t>
   </si>
   <si>
@@ -132,6 +130,105 @@
   </si>
   <si>
     <t>rudraksh@igtsolutions.com</t>
+  </si>
+  <si>
+    <t>ConfirmationCode</t>
+  </si>
+  <si>
+    <t>RoomBefore</t>
+  </si>
+  <si>
+    <t>RoomAfter</t>
+  </si>
+  <si>
+    <t>DatesBefore</t>
+  </si>
+  <si>
+    <t>DatesAfter</t>
+  </si>
+  <si>
+    <t>NoOfAdultAndChildBefore</t>
+  </si>
+  <si>
+    <t>NoOfAdultAndChildAfter</t>
+  </si>
+  <si>
+    <t>GuestDetailsBefore</t>
+  </si>
+  <si>
+    <t>GuestDetailsAfter</t>
+  </si>
+  <si>
+    <t>BedTypeBefore</t>
+  </si>
+  <si>
+    <t>BedTypeAfter</t>
+  </si>
+  <si>
+    <t>OtherServicesBefore</t>
+  </si>
+  <si>
+    <t>OtherServicesAfter</t>
+  </si>
+  <si>
+    <t>Standard Room</t>
+  </si>
+  <si>
+    <t>ALH100002653</t>
+  </si>
+  <si>
+    <t>Thu, 2022-02-10➝Fri, 2022-02-11</t>
+  </si>
+  <si>
+    <t>Thu, 2022-02-10➝Sat, 2022-02-12</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>rudraksh aggarwal</t>
+  </si>
+  <si>
+    <t>john smith</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Classic Bed type</t>
+  </si>
+  <si>
+    <t>$0.00</t>
+  </si>
+  <si>
+    <t>$10.00</t>
+  </si>
+  <si>
+    <t>0</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>Adults</t>
+  </si>
+  <si>
+    <t>Children</t>
+  </si>
+  <si>
+    <t>Child</t>
+  </si>
+  <si>
+    <t>3 adults</t>
+  </si>
+  <si>
+    <t>john</t>
+  </si>
+  <si>
+    <t>smith</t>
   </si>
 </sst>
 </file>
@@ -461,29 +558,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S5"/>
+  <dimension ref="A1:AF5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="N1" workbookViewId="0">
-      <selection activeCell="Q15" sqref="Q15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="44.5703125" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="10" width="17.42578125" customWidth="1"/>
-    <col min="11" max="12" width="11.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="36.85546875" customWidth="1"/>
+    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="13.85546875" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="9" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="32.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="10" width="12.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="12" width="11.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="5.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="13" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="16" max="17" width="16.5703125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="6.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="24" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="16.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="13.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="22" max="22" width="11.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="23" max="23" width="28.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="24" max="24" width="29.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="25" max="25" width="23" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="26" max="26" width="21.5703125" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -536,18 +642,57 @@
         <v>29</v>
       </c>
       <c r="R1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="S1" t="s">
-        <v>33</v>
+        <v>32</v>
+      </c>
+      <c r="T1" t="s">
+        <v>35</v>
+      </c>
+      <c r="U1" t="s">
+        <v>36</v>
+      </c>
+      <c r="V1" t="s">
+        <v>37</v>
+      </c>
+      <c r="W1" t="s">
+        <v>38</v>
+      </c>
+      <c r="X1" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>48</v>
       </c>
       <c r="C2" t="s">
         <v>20</v>
@@ -556,7 +701,7 @@
         <v>9</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F2" t="s">
         <v>5</v>
@@ -592,28 +737,73 @@
         <v>18</v>
       </c>
       <c r="Q2" t="s">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="R2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
+      </c>
+      <c r="T2" t="s">
+        <v>49</v>
+      </c>
+      <c r="U2" t="s">
+        <v>48</v>
+      </c>
+      <c r="V2" t="s">
+        <v>3</v>
+      </c>
+      <c r="W2" t="s">
+        <v>50</v>
+      </c>
+      <c r="X2" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>52</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>55</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="G3" s="1"/>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
+      <c r="Y3" t="s">
+        <v>60</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>61</v>
+      </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="G4" s="1"/>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
@@ -626,4 +816,59 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="10.85546875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="10.140625" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12.85546875" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="17" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" t="s">
+        <v>64</v>
+      </c>
+      <c r="D1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E2" t="s">
+        <v>67</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Booking Engine Script Updated
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/CC_CallCenterData.xlsx
+++ b/src/test/resources/testData/CC_CallCenterData.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" firstSheet="29" activeTab="33"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" firstSheet="30" activeTab="33"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPageData" sheetId="1" r:id="rId1"/>
@@ -46,6 +46,7 @@
     <sheet name="Booking" sheetId="36" r:id="rId32"/>
     <sheet name="NormalSingleRoomBookingData" sheetId="37" r:id="rId33"/>
     <sheet name="MobileB" sheetId="38" r:id="rId34"/>
+    <sheet name="Sheet2" sheetId="39" r:id="rId35"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -57,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="679" uniqueCount="491">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="715" uniqueCount="506">
   <si>
     <t>Username</t>
   </si>
@@ -1520,16 +1521,61 @@
     <t>CCode</t>
   </si>
   <si>
+    <t>Country</t>
+  </si>
+  <si>
+    <t>India</t>
+  </si>
+  <si>
+    <t>Dk</t>
+  </si>
+  <si>
+    <t>7883664742</t>
+  </si>
+  <si>
+    <t>Chennai</t>
+  </si>
+  <si>
+    <t>Tamil Nadu</t>
+  </si>
+  <si>
+    <t>600064</t>
+  </si>
+  <si>
+    <t>222</t>
+  </si>
+  <si>
+    <t>4012 8888 8888 1881</t>
+  </si>
+  <si>
+    <t>11/22</t>
+  </si>
+  <si>
     <t>AnkitaM</t>
   </si>
   <si>
     <t>ankita.mohamanasingh@pegs.com</t>
   </si>
   <si>
-    <t>5454545454545454</t>
+    <t>123456789</t>
+  </si>
+  <si>
+    <t>123456</t>
+  </si>
+  <si>
+    <t>5454</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>28</t>
   </si>
   <si>
     <t>Administrator</t>
+  </si>
+  <si>
+    <t>Call center Ale hotel</t>
   </si>
 </sst>
 </file>
@@ -1586,7 +1632,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
@@ -1606,6 +1652,7 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1895,13 +1942,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="16.42578125" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="15.5703125" collapsed="false"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="13.140625" collapsed="false"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="26.5703125" collapsed="false"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="16.42578125" collapsed="false"/>
-    <col min="6" max="6" customWidth="true" width="15.85546875" collapsed="false"/>
-    <col min="7" max="7" customWidth="true" width="18.140625" collapsed="false"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="16.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="26.5703125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="16.42578125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="18.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
@@ -1971,7 +2018,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="22.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" customWidth="true" width="24.85546875" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" width="24.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
@@ -2083,9 +2130,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" bestFit="true" customWidth="true" width="10.140625" collapsed="false"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="10.140625" collapsed="false"/>
-    <col min="7" max="7" customWidth="true" width="13.5703125" collapsed="false"/>
+    <col min="1" max="2" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="13.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -2161,7 +2208,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" customWidth="true" width="16.42578125" collapsed="false"/>
+    <col min="3" max="3" customWidth="true" width="16.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -2201,30 +2248,30 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="17.28515625" collapsed="false"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="15.0" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" width="13.42578125" collapsed="false"/>
-    <col min="4" max="4" customWidth="true" width="16.28515625" collapsed="false"/>
-    <col min="5" max="5" customWidth="true" width="15.42578125" collapsed="false"/>
-    <col min="7" max="7" customWidth="true" width="15.140625" collapsed="false"/>
-    <col min="10" max="10" customWidth="true" width="20.140625" collapsed="false"/>
-    <col min="11" max="11" customWidth="true" width="11.7109375" collapsed="false"/>
-    <col min="12" max="12" customWidth="true" width="16.28515625" collapsed="false"/>
-    <col min="13" max="13" customWidth="true" width="33.0" collapsed="false"/>
-    <col min="14" max="14" customWidth="true" width="13.85546875" collapsed="false"/>
-    <col min="15" max="15" customWidth="true" width="37.42578125" collapsed="false"/>
-    <col min="16" max="16" customWidth="true" width="14.28515625" collapsed="false"/>
-    <col min="17" max="17" customWidth="true" width="11.5703125" collapsed="false"/>
-    <col min="18" max="18" customWidth="true" width="18.5703125" collapsed="false"/>
-    <col min="19" max="20" bestFit="true" customWidth="true" width="10.7109375" collapsed="false"/>
-    <col min="21" max="21" customWidth="true" width="17.0" collapsed="false"/>
-    <col min="22" max="22" customWidth="true" width="43.5703125" collapsed="false"/>
-    <col min="23" max="23" customWidth="true" width="18.140625" collapsed="false"/>
-    <col min="24" max="24" customWidth="true" width="17.42578125" collapsed="false"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="10.28515625" collapsed="false"/>
-    <col min="26" max="26" customWidth="true" width="10.28515625" collapsed="false"/>
-    <col min="27" max="27" customWidth="true" width="14.5703125" collapsed="false"/>
-    <col min="28" max="28" customWidth="true" width="15.85546875" collapsed="false"/>
+    <col min="1" max="1" customWidth="true" width="17.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="20.140625" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="33.0" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="37.42578125" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="19" max="20" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="21" max="21" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" width="43.5703125" collapsed="true"/>
+    <col min="23" max="23" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="24" max="24" customWidth="true" width="17.42578125" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="26" max="26" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="27" max="27" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="28" max="28" customWidth="true" width="15.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.25">
@@ -2586,8 +2633,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="11.5703125" collapsed="false"/>
-    <col min="5" max="5" customWidth="true" width="11.5703125" collapsed="false"/>
+    <col min="1" max="1" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="11.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:25" x14ac:dyDescent="0.25">
@@ -2738,16 +2785,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="15.85546875" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" width="13.28515625" collapsed="false"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="15.85546875" collapsed="false"/>
-    <col min="6" max="6" customWidth="true" width="13.0" collapsed="false"/>
-    <col min="7" max="7" customWidth="true" width="15.5703125" collapsed="false"/>
-    <col min="9" max="9" customWidth="true" width="14.85546875" collapsed="false"/>
-    <col min="10" max="10" customWidth="true" width="15.28515625" collapsed="false"/>
-    <col min="12" max="12" customWidth="true" width="13.42578125" collapsed="false"/>
-    <col min="13" max="13" customWidth="true" width="15.42578125" collapsed="false"/>
-    <col min="14" max="14" customWidth="true" width="15.5703125" collapsed="false"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="15.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
@@ -2859,13 +2906,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="15.85546875" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" width="14.5703125" collapsed="false"/>
-    <col min="4" max="4" customWidth="true" width="15.28515625" collapsed="false"/>
-    <col min="5" max="5" customWidth="true" width="13.7109375" collapsed="false"/>
-    <col min="6" max="6" customWidth="true" width="15.85546875" collapsed="false"/>
-    <col min="8" max="8" customWidth="true" width="14.0" collapsed="false"/>
-    <col min="9" max="9" customWidth="true" width="13.140625" collapsed="false"/>
+    <col min="1" max="1" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -2941,18 +2988,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="19.140625" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" width="13.85546875" collapsed="false"/>
-    <col min="4" max="4" customWidth="true" width="12.0" collapsed="false"/>
-    <col min="6" max="6" customWidth="true" width="13.140625" collapsed="false"/>
-    <col min="7" max="7" customWidth="true" width="14.140625" collapsed="false"/>
-    <col min="9" max="9" customWidth="true" width="15.28515625" collapsed="false"/>
-    <col min="10" max="10" customWidth="true" width="16.140625" collapsed="false"/>
-    <col min="12" max="12" customWidth="true" width="13.5703125" collapsed="false"/>
-    <col min="13" max="13" customWidth="true" width="16.28515625" collapsed="false"/>
-    <col min="15" max="15" customWidth="true" width="14.5703125" collapsed="false"/>
-    <col min="16" max="16" customWidth="true" width="13.42578125" collapsed="false"/>
-    <col min="18" max="18" customWidth="true" width="14.140625" collapsed="false"/>
+    <col min="1" max="1" customWidth="true" width="19.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="13.5703125" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" width="14.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -3046,13 +3093,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="13.5703125" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" width="14.28515625" collapsed="false"/>
-    <col min="4" max="4" customWidth="true" width="12.140625" collapsed="false"/>
-    <col min="6" max="6" customWidth="true" width="13.85546875" collapsed="false"/>
-    <col min="7" max="7" customWidth="true" width="14.5703125" collapsed="false"/>
-    <col min="9" max="9" customWidth="true" width="13.140625" collapsed="false"/>
-    <col min="10" max="10" customWidth="true" width="18.5703125" collapsed="false"/>
+    <col min="1" max="1" customWidth="true" width="13.5703125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="12.140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="18.5703125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -3134,14 +3181,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="15.140625" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" width="12.85546875" collapsed="false"/>
-    <col min="4" max="4" customWidth="true" width="15.140625" collapsed="false"/>
-    <col min="6" max="6" customWidth="true" width="13.7109375" collapsed="false"/>
-    <col min="7" max="7" customWidth="true" width="15.42578125" collapsed="false"/>
-    <col min="9" max="9" customWidth="true" width="15.140625" collapsed="false"/>
-    <col min="12" max="12" customWidth="true" width="14.85546875" collapsed="false"/>
-    <col min="13" max="13" customWidth="true" width="19.140625" collapsed="false"/>
+    <col min="1" max="1" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="19.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -3272,17 +3319,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="11.42578125" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="10.140625" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" width="13.85546875" collapsed="false"/>
-    <col min="4" max="4" customWidth="true" width="13.140625" collapsed="false"/>
-    <col min="5" max="5" customWidth="true" width="9.7109375" collapsed="false"/>
-    <col min="6" max="6" customWidth="true" width="14.85546875" collapsed="false"/>
-    <col min="7" max="7" customWidth="true" width="10.42578125" collapsed="false"/>
-    <col min="8" max="8" customWidth="true" width="9.85546875" collapsed="false"/>
-    <col min="9" max="9" customWidth="true" width="14.5703125" collapsed="false"/>
-    <col min="10" max="10" customWidth="true" width="20.0" collapsed="false"/>
-    <col min="11" max="11" customWidth="true" width="13.140625" collapsed="false"/>
+    <col min="1" max="1" customWidth="true" width="11.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="9.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="10.42578125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="9.85546875" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="13.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -3380,12 +3427,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="14.28515625" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" width="13.5703125" collapsed="false"/>
-    <col min="4" max="4" customWidth="true" width="15.5703125" collapsed="false"/>
-    <col min="6" max="6" customWidth="true" width="13.85546875" collapsed="false"/>
-    <col min="7" max="7" customWidth="true" width="14.7109375" collapsed="false"/>
-    <col min="9" max="9" customWidth="true" width="14.0" collapsed="false"/>
+    <col min="1" max="1" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="13.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="14.7109375" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="14.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -3600,23 +3647,23 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="10.85546875" collapsed="false"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.5703125" collapsed="false"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="15.7109375" collapsed="false"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="9.5703125" collapsed="false"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="9.85546875" collapsed="false"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="15.5703125" collapsed="false"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="18.0" collapsed="false"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="9.28515625" collapsed="false"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="9.0" collapsed="false"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="32.140625" collapsed="false"/>
-    <col min="11" max="12" bestFit="true" customWidth="true" width="11.5703125" collapsed="false"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="5.140625" collapsed="false"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="7.28515625" collapsed="false"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="13.0" collapsed="false"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="10.42578125" collapsed="false"/>
-    <col min="17" max="20" bestFit="true" customWidth="true" width="12.5703125" collapsed="false"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="18.42578125" collapsed="false"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="10.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="9.5703125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="9.28515625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="32.140625" collapsed="true"/>
+    <col min="11" max="12" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="5.140625" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
+    <col min="17" max="20" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="18.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.25">
@@ -3782,8 +3829,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.5703125" collapsed="false"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="15.0" collapsed="false"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -3817,12 +3864,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="10.0" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="13.28515625" collapsed="false"/>
-    <col min="5" max="5" customWidth="true" width="39.140625" collapsed="false"/>
-    <col min="6" max="6" customWidth="true" width="10.42578125" collapsed="false"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="19.5703125" collapsed="false"/>
-    <col min="11" max="11" customWidth="true" width="12.85546875" collapsed="false"/>
+    <col min="1" max="1" customWidth="true" width="10.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="39.140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="10.42578125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="19.5703125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="12.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -3920,11 +3967,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="11.42578125" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="13.5703125" collapsed="false"/>
-    <col min="5" max="5" customWidth="true" width="37.85546875" collapsed="false"/>
-    <col min="7" max="7" customWidth="true" width="16.42578125" collapsed="false"/>
-    <col min="13" max="13" customWidth="true" width="21.28515625" collapsed="false"/>
+    <col min="1" max="1" customWidth="true" width="11.42578125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="13.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="37.85546875" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="16.42578125" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="21.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -4027,10 +4074,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="12.5703125" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="13.85546875" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" width="10.140625" collapsed="false"/>
-    <col min="4" max="4" customWidth="true" width="9.42578125" collapsed="false"/>
+    <col min="1" max="1" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="13.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="9.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -4127,10 +4174,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="11.5703125" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="14.28515625" collapsed="false"/>
-    <col min="5" max="5" customWidth="true" width="36.5703125" collapsed="false"/>
-    <col min="11" max="11" customWidth="true" width="10.7109375" collapsed="false"/>
+    <col min="1" max="1" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="14.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="36.5703125" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="10.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -4264,20 +4311,20 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="6.28515625" collapsed="false"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="5.5703125" collapsed="false"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.140625" collapsed="false"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="37.5703125" collapsed="false"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="12.7109375" collapsed="false"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="9.28515625" collapsed="false"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="12.5703125" collapsed="false"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="9.7109375" collapsed="false"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="11.5703125" collapsed="false"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="21.42578125" collapsed="false"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="26.5703125" collapsed="false"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="16.5703125" collapsed="false"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="16.0" collapsed="false"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="21.42578125" collapsed="false"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="6.28515625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="5.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="37.5703125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="9.28515625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="12.5703125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="9.7109375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="21.42578125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="26.5703125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="16.5703125" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="21.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -4448,11 +4495,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="16.5703125" collapsed="false"/>
-    <col min="2" max="2" customWidth="true" width="11.7109375" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" width="11.0" collapsed="false"/>
-    <col min="4" max="4" customWidth="true" width="10.42578125" collapsed="false"/>
-    <col min="5" max="5" customWidth="true" width="12.28515625" collapsed="false"/>
+    <col min="1" max="1" customWidth="true" width="16.5703125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.42578125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -4504,18 +4551,18 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="13.42578125" collapsed="false"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="11.28515625" collapsed="false"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="9.28515625" collapsed="false"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="9.0" collapsed="false"/>
-    <col min="5" max="5" customWidth="true" width="44.5703125" collapsed="false"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="10.7109375" collapsed="false"/>
-    <col min="7" max="10" customWidth="true" width="17.42578125" collapsed="false"/>
-    <col min="11" max="12" bestFit="true" customWidth="true" width="11.5703125" collapsed="false"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="5.140625" collapsed="false"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="7.28515625" collapsed="false"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="13.0" collapsed="false"/>
-    <col min="19" max="19" customWidth="true" width="36.85546875" collapsed="false"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.28515625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="9.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="44.5703125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="7" max="10" customWidth="true" width="17.42578125" collapsed="true"/>
+    <col min="11" max="12" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="5.140625" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" width="36.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:19" x14ac:dyDescent="0.25">
@@ -4636,10 +4683,10 @@
         <v>479</v>
       </c>
       <c r="AH2" t="s">
-        <v>490</v>
+        <v>505</v>
       </c>
       <c r="AI2" t="s">
-        <v>490</v>
+        <v>504</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
@@ -4671,20 +4718,21 @@
 
 <file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:K5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="9.85546875" collapsed="false"/>
-    <col min="3" max="3" customWidth="true" width="30.140625" collapsed="false"/>
-    <col min="8" max="8" customWidth="true" width="16.42578125" collapsed="false"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="30.140625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="17.28515625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>482</v>
       </c>
@@ -4715,16 +4763,19 @@
       <c r="J1" t="s">
         <v>486</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K1" t="s">
+        <v>487</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>487</v>
-      </c>
-      <c r="B2">
-        <v>123456789</v>
+        <v>497</v>
+      </c>
+      <c r="B2" t="s">
+        <v>499</v>
       </c>
       <c r="C2" t="s">
-        <v>488</v>
+        <v>498</v>
       </c>
       <c r="D2" t="s">
         <v>414</v>
@@ -4735,17 +4786,130 @@
       <c r="F2" t="s">
         <v>414</v>
       </c>
-      <c r="G2">
-        <v>123456</v>
+      <c r="G2" s="3" t="s">
+        <v>500</v>
       </c>
       <c r="H2" s="3" t="s">
+        <v>501</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>502</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="K2" t="s">
+        <v>488</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H3" s="3" t="s">
+        <v>501</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>503</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H4" s="3" t="s">
+        <v>501</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="H5" s="3" t="s">
+        <v>501</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="30.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>482</v>
+      </c>
+      <c r="B1" t="s">
+        <v>436</v>
+      </c>
+      <c r="C1" t="s">
+        <v>398</v>
+      </c>
+      <c r="D1" t="s">
+        <v>151</v>
+      </c>
+      <c r="E1" t="s">
+        <v>487</v>
+      </c>
+      <c r="F1" t="s">
+        <v>483</v>
+      </c>
+      <c r="G1" t="s">
+        <v>104</v>
+      </c>
+      <c r="H1" t="s">
+        <v>437</v>
+      </c>
+      <c r="I1" t="s">
+        <v>484</v>
+      </c>
+      <c r="J1" t="s">
+        <v>485</v>
+      </c>
+      <c r="K1" t="s">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>489</v>
       </c>
-      <c r="I2">
-        <v>1112</v>
-      </c>
-      <c r="J2">
-        <v>123</v>
+      <c r="B2" s="3" t="s">
+        <v>490</v>
+      </c>
+      <c r="C2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D2" t="s">
+        <v>491</v>
+      </c>
+      <c r="E2" t="s">
+        <v>488</v>
+      </c>
+      <c r="F2" t="s">
+        <v>492</v>
+      </c>
+      <c r="G2" t="s">
+        <v>491</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>493</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>495</v>
+      </c>
+      <c r="J2" s="17" t="s">
+        <v>496</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>494</v>
       </c>
     </row>
   </sheetData>
@@ -4812,11 +4976,11 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.5703125" collapsed="false"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="20.0" collapsed="false"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="19.140625" collapsed="false"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="24.85546875" collapsed="false"/>
-    <col min="8" max="8" customWidth="true" width="34.0" collapsed="false"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="19.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="24.85546875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="34.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -4944,18 +5108,18 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="10.85546875" collapsed="false"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="10.140625" collapsed="false"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="20.0" collapsed="false"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="9.85546875" collapsed="false"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="10.85546875" collapsed="false"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="10.140625" collapsed="false"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="20.0" collapsed="false"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="9.85546875" collapsed="false"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="10.85546875" collapsed="false"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="10.140625" collapsed="false"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="20.0" collapsed="false"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="9.85546875" collapsed="false"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="10.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="10.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="10.85546875" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="10.140625" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="20.0" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
@@ -5049,8 +5213,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="13.140625" collapsed="false"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="18.42578125" collapsed="false"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="18.42578125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
CC Excel sheet updated
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/CC_CallCenterData.xlsx
+++ b/src/test/resources/testData/CC_CallCenterData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14350" windowHeight="4240" tabRatio="667"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14530" windowHeight="2990" tabRatio="793"/>
   </bookViews>
   <sheets>
     <sheet name="NormalSingleRoomBookingData" sheetId="1" r:id="rId1"/>
@@ -17,14 +17,16 @@
     <sheet name="rt3bookingcctobeviceversa" sheetId="10" r:id="rId8"/>
     <sheet name="OfferAccessCodeBooking" sheetId="11" r:id="rId9"/>
     <sheet name="FiltersData" sheetId="12" r:id="rId10"/>
+    <sheet name="MultiRoomBookingRateGridUpdate" sheetId="13" r:id="rId11"/>
+    <sheet name="AlternateCurrencyBookings" sheetId="14" r:id="rId12"/>
   </sheets>
   <calcPr calcId="0"/>
-  <oleSize ref="AY1:BD12"/>
+  <oleSize ref="N1:V8"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="217">
   <si>
     <t>RoomAvailable</t>
   </si>
@@ -275,9 +277,6 @@
     <t>abraham</t>
   </si>
   <si>
-    <t>Call center Ale hotel</t>
-  </si>
-  <si>
     <t>Administrator</t>
   </si>
   <si>
@@ -527,9 +526,6 @@
     <t>ALH100003951</t>
   </si>
   <si>
-    <t>ALH100003969</t>
-  </si>
-  <si>
     <t>BedName</t>
   </si>
   <si>
@@ -540,13 +536,155 @@
   </si>
   <si>
     <t>TBT</t>
+  </si>
+  <si>
+    <t>number:2</t>
+  </si>
+  <si>
+    <t>NoOfRooms</t>
+  </si>
+  <si>
+    <t>ExpAvailTC01</t>
+  </si>
+  <si>
+    <t>98</t>
+  </si>
+  <si>
+    <t>Grande Penthouse</t>
+  </si>
+  <si>
+    <t>number:3</t>
+  </si>
+  <si>
+    <t>Z_TestRoom</t>
+  </si>
+  <si>
+    <t>RoomCode</t>
+  </si>
+  <si>
+    <t>ztr</t>
+  </si>
+  <si>
+    <t>ExtraAdultChargePerRoom</t>
+  </si>
+  <si>
+    <t>ExtraChildChargePerRoom</t>
+  </si>
+  <si>
+    <t>150</t>
+  </si>
+  <si>
+    <t>20</t>
+  </si>
+  <si>
+    <t>minAdult</t>
+  </si>
+  <si>
+    <t>maxAdult</t>
+  </si>
+  <si>
+    <t>minChild</t>
+  </si>
+  <si>
+    <t>maxChild</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>Occ</t>
+  </si>
+  <si>
+    <t>United States Dollar</t>
+  </si>
+  <si>
+    <t>DefaultCurrencyAdmin</t>
+  </si>
+  <si>
+    <t>CurrencyCC</t>
+  </si>
+  <si>
+    <t>DefaultCurrencyCC</t>
+  </si>
+  <si>
+    <t>Indian Rupee</t>
+  </si>
+  <si>
+    <t>AlternateCurrencyAdmin</t>
+  </si>
+  <si>
+    <t>AlternateCurrencyCC</t>
+  </si>
+  <si>
+    <t>INR</t>
+  </si>
+  <si>
+    <t>ChargeTC02_1</t>
+  </si>
+  <si>
+    <t>ChargeTC02_2</t>
+  </si>
+  <si>
+    <t>ChargeTC03_1</t>
+  </si>
+  <si>
+    <t>ChargeTC03_2</t>
+  </si>
+  <si>
+    <t>ChargeTC04_1</t>
+  </si>
+  <si>
+    <t>ChargeTC04_2</t>
+  </si>
+  <si>
+    <t>ChargeTC05_1</t>
+  </si>
+  <si>
+    <t>ChargeTC05_2</t>
+  </si>
+  <si>
+    <t>ALH100004621</t>
+  </si>
+  <si>
+    <t>$170.00 /night</t>
+  </si>
+  <si>
+    <t>INR12,962.30 /night</t>
+  </si>
+  <si>
+    <t>INR12,962.30</t>
+  </si>
+  <si>
+    <t>$170.00</t>
+  </si>
+  <si>
+    <t>ALH100004631</t>
+  </si>
+  <si>
+    <t>INR170.00</t>
+  </si>
+  <si>
+    <t>INR12,975.93 /night</t>
+  </si>
+  <si>
+    <t>INR12,975.93</t>
+  </si>
+  <si>
+    <t>ALH100004680</t>
+  </si>
+  <si>
+    <t>ALH100004684</t>
+  </si>
+  <si>
+    <t>ALH100004686</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3">
+  <numFmts count="0"/>
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -555,17 +693,45 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="9"/>
       <color rgb="FF202124"/>
       <name val="Consolas"/>
-      <charset val="134"/>
+      <family val="3"/>
     </font>
     <font>
       <u/>
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -588,13 +754,17 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -871,42 +1041,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BD4"/>
+  <dimension ref="A1:BQ4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="BM1" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="BQ4" sqref="BQ4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.6328125" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="13.36328125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="13.81640625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="9.26953125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="9" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="32.1796875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="10.7265625" customWidth="1" collapsed="1"/>
-    <col min="7" max="10" width="12.54296875" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="11.6328125" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="11.54296875" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="5.08984375" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="7.26953125" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="13" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="16.54296875" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="16.6328125" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="6.81640625" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="24" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="16.1796875" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="13.81640625" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="11.26953125" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="28.81640625" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="29.36328125" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="23" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="21.6328125" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="29.7265625" customWidth="1" collapsed="1"/>
-    <col min="43" max="43" width="29.1796875" customWidth="1" collapsed="1"/>
-    <col min="51" max="51" width="23.81640625" customWidth="1" collapsed="1"/>
-    <col min="54" max="54" width="23.81640625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="13.36328125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="13.81640625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="9.26953125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="9.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="32.1796875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="10.7265625" collapsed="true"/>
+    <col min="7" max="10" customWidth="true" width="12.54296875" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="11.6328125" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="11.54296875" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="5.08984375" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="7.26953125" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="13.0" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="16.54296875" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="16.6328125" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" width="6.81640625" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" width="24.0" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" width="16.1796875" collapsed="true"/>
+    <col min="21" max="21" customWidth="true" width="13.81640625" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" width="11.26953125" collapsed="true"/>
+    <col min="23" max="23" customWidth="true" width="28.81640625" collapsed="true"/>
+    <col min="24" max="24" customWidth="true" width="29.36328125" collapsed="true"/>
+    <col min="25" max="25" customWidth="true" width="23.0" collapsed="true"/>
+    <col min="26" max="26" customWidth="true" width="21.6328125" collapsed="true"/>
+    <col min="39" max="39" customWidth="true" width="29.7265625" collapsed="true"/>
+    <col min="43" max="43" customWidth="true" width="29.1796875" collapsed="true"/>
+    <col min="51" max="51" customWidth="true" width="23.81640625" collapsed="true"/>
+    <col min="54" max="54" customWidth="true" width="23.81640625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:56">
+    <row r="1" spans="1:69">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1075,8 +1247,45 @@
       <c r="BD1" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="2" spans="1:56">
+      <c r="BE1" t="s">
+        <v>190</v>
+      </c>
+      <c r="BF1" t="s">
+        <v>192</v>
+      </c>
+      <c r="BG1" t="s">
+        <v>194</v>
+      </c>
+      <c r="BH1" t="s">
+        <v>195</v>
+      </c>
+      <c r="BI1" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="BJ1" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="BK1" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="BL1" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="BM1" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="BN1" s="6" t="s">
+        <v>202</v>
+      </c>
+      <c r="BO1" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="BP1" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="BQ1" s="7"/>
+    </row>
+    <row r="2" spans="1:69">
       <c r="A2" s="3" t="s">
         <v>56</v>
       </c>
@@ -1135,7 +1344,7 @@
         <v>72</v>
       </c>
       <c r="T2" t="s">
-        <v>167</v>
+        <v>216</v>
       </c>
       <c r="U2" t="s">
         <v>57</v>
@@ -1147,7 +1356,7 @@
         <v>73</v>
       </c>
       <c r="X2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="Y2" t="s">
         <v>74</v>
@@ -1180,19 +1389,19 @@
         <v>83</v>
       </c>
       <c r="AI2" t="s">
+        <v>83</v>
+      </c>
+      <c r="AJ2" t="s">
         <v>84</v>
       </c>
-      <c r="AJ2" t="s">
+      <c r="AK2" t="s">
         <v>85</v>
       </c>
-      <c r="AK2" t="s">
-        <v>86</v>
-      </c>
       <c r="AL2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="AM2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="AN2" t="s">
         <v>57</v>
@@ -1201,80 +1410,119 @@
         <v>70</v>
       </c>
       <c r="AP2" t="s">
+        <v>86</v>
+      </c>
+      <c r="AQ2" t="s">
+        <v>162</v>
+      </c>
+      <c r="AR2" t="s">
         <v>87</v>
       </c>
-      <c r="AQ2" t="s">
-        <v>163</v>
-      </c>
-      <c r="AR2" t="s">
+      <c r="AS2" t="s">
         <v>88</v>
       </c>
-      <c r="AS2" t="s">
+      <c r="AT2" t="s">
         <v>89</v>
       </c>
-      <c r="AT2" t="s">
+      <c r="AU2" t="s">
         <v>90</v>
       </c>
-      <c r="AU2" t="s">
+      <c r="AV2" t="s">
+        <v>90</v>
+      </c>
+      <c r="AW2" t="s">
+        <v>89</v>
+      </c>
+      <c r="AX2" t="s">
         <v>91</v>
       </c>
-      <c r="AV2" t="s">
-        <v>91</v>
-      </c>
-      <c r="AW2" t="s">
-        <v>90</v>
-      </c>
-      <c r="AX2" t="s">
+      <c r="AY2" t="s">
         <v>92</v>
       </c>
-      <c r="AY2" t="s">
+      <c r="AZ2" t="s">
         <v>93</v>
       </c>
-      <c r="AZ2" t="s">
+      <c r="BA2" t="s">
         <v>94</v>
       </c>
-      <c r="BA2" t="s">
+      <c r="BB2" t="s">
         <v>95</v>
       </c>
-      <c r="BB2" t="s">
+      <c r="BC2" t="s">
         <v>96</v>
-      </c>
-      <c r="BC2" t="s">
-        <v>97</v>
       </c>
       <c r="BD2" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="3" spans="1:56">
+      <c r="BE2" t="s">
+        <v>189</v>
+      </c>
+      <c r="BF2" t="s">
+        <v>150</v>
+      </c>
+      <c r="BG2" t="s">
+        <v>193</v>
+      </c>
+      <c r="BH2" t="s">
+        <v>196</v>
+      </c>
+      <c r="BI2" t="s">
+        <v>206</v>
+      </c>
+      <c r="BJ2" t="s">
+        <v>212</v>
+      </c>
+      <c r="BK2" t="s">
+        <v>213</v>
+      </c>
+      <c r="BL2" t="s">
+        <v>209</v>
+      </c>
+      <c r="BM2" t="s">
+        <v>209</v>
+      </c>
+      <c r="BN2" t="s">
+        <v>213</v>
+      </c>
+      <c r="BO2" t="s">
+        <v>209</v>
+      </c>
+      <c r="BP2" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="3" spans="1:69">
       <c r="A3" t="s">
-        <v>92</v>
+        <v>91</v>
+      </c>
+      <c r="B3" t="s">
+        <v>174</v>
       </c>
       <c r="Y3" t="s">
+        <v>97</v>
+      </c>
+      <c r="Z3" t="s">
         <v>98</v>
       </c>
-      <c r="Z3" t="s">
+      <c r="AK3" t="s">
         <v>99</v>
       </c>
-      <c r="AK3" t="s">
+      <c r="AZ3" t="s">
         <v>100</v>
       </c>
-      <c r="AZ3" t="s">
+      <c r="BA3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4" spans="1:69">
+      <c r="AK4" t="s">
         <v>101</v>
       </c>
-      <c r="BA3" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="4" spans="1:56">
-      <c r="AK4" t="s">
+      <c r="AZ4" t="s">
         <v>102</v>
       </c>
-      <c r="AZ4" t="s">
-        <v>103</v>
-      </c>
       <c r="BA4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -1283,6 +1531,7 @@
     <hyperlink ref="S2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -1296,64 +1545,64 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="16.1796875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="29.453125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="11.7265625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="9.36328125" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="16.1796875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="29.453125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="11.7265625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="9.36328125" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B1" t="s">
+        <v>155</v>
+      </c>
+      <c r="C1" t="s">
         <v>156</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
+        <v>138</v>
+      </c>
+      <c r="E1" t="s">
         <v>157</v>
       </c>
-      <c r="D1" t="s">
-        <v>139</v>
-      </c>
-      <c r="E1" t="s">
-        <v>158</v>
-      </c>
       <c r="F1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="G1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
+        <v>158</v>
+      </c>
+      <c r="B2" t="s">
+        <v>96</v>
+      </c>
+      <c r="C2" t="s">
         <v>159</v>
       </c>
-      <c r="B2" t="s">
-        <v>97</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D2" s="3" t="s">
         <v>160</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>161</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>70</v>
       </c>
       <c r="F2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G2" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="3" spans="1:7">
       <c r="B3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
   </sheetData>
@@ -1361,31 +1610,191 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="13.54296875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="22.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="25.90625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="23.0" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" t="s">
+        <v>171</v>
+      </c>
+      <c r="B1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>177</v>
+      </c>
+      <c r="E1" t="s">
+        <v>179</v>
+      </c>
+      <c r="F1" t="s">
+        <v>180</v>
+      </c>
+      <c r="G1" t="s">
+        <v>183</v>
+      </c>
+      <c r="H1" t="s">
+        <v>184</v>
+      </c>
+      <c r="I1" t="s">
+        <v>185</v>
+      </c>
+      <c r="J1" t="s">
+        <v>186</v>
+      </c>
+      <c r="K1" t="s">
+        <v>188</v>
+      </c>
+      <c r="L1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12">
+      <c r="A2" t="s">
+        <v>170</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="C2" t="s">
+        <v>176</v>
+      </c>
+      <c r="D2" t="s">
+        <v>178</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" t="s">
+        <v>175</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5"/>
+  <cols>
+    <col min="1" max="1" customWidth="true" width="23.1796875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="13.26953125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="27.1796875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="27.81640625" collapsed="true"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B1" t="s">
+        <v>191</v>
+      </c>
+      <c r="C1" t="s">
+        <v>194</v>
+      </c>
+      <c r="D1" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>189</v>
+      </c>
+      <c r="B2" t="s">
+        <v>150</v>
+      </c>
+      <c r="C2" t="s">
+        <v>193</v>
+      </c>
+      <c r="D2" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C3" t="s">
+        <v>196</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
-    <col min="4" max="4" width="10.81640625" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="10.1796875" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="12.81640625" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="17" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" customWidth="true" width="10.81640625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="10.1796875" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="12.81640625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="17.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B1" t="s">
         <v>104</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>105</v>
-      </c>
-      <c r="C1" t="s">
-        <v>106</v>
       </c>
       <c r="D1" t="s">
         <v>2</v>
@@ -1396,19 +1805,19 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" t="s">
+        <v>106</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D2" t="s">
         <v>107</v>
       </c>
-      <c r="B2" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>108</v>
-      </c>
-      <c r="E2" t="s">
-        <v>109</v>
       </c>
     </row>
   </sheetData>
@@ -1420,38 +1829,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="13.453125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="13.1796875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.453125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="13.1796875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="13.453125" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="13.1796875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="13.453125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="13.1796875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="13.453125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="13.1796875" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="13.453125" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="13.1796875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B1" t="s">
         <v>110</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>111</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>112</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>113</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>114</v>
-      </c>
-      <c r="F1" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="2" spans="1:6">
@@ -1459,16 +1868,16 @@
         <v>71</v>
       </c>
       <c r="B2" t="s">
+        <v>115</v>
+      </c>
+      <c r="C2" t="s">
         <v>116</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>117</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>118</v>
-      </c>
-      <c r="E2" t="s">
-        <v>119</v>
       </c>
       <c r="F2" t="s">
         <v>82</v>
@@ -1483,44 +1892,44 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="28.90625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="22.7265625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14.453125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="10.1796875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="28.90625" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="22.7265625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="14.453125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="10.1796875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B1" t="s">
         <v>120</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>121</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>122</v>
-      </c>
-      <c r="D1" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" t="s">
         <v>125</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>126</v>
-      </c>
-      <c r="D2" t="s">
-        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -1535,28 +1944,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="32.6328125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="9" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="32.6328125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="9.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B1" t="s">
         <v>128</v>
-      </c>
-      <c r="B1" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
+        <v>129</v>
+      </c>
+      <c r="B2" t="s">
         <v>130</v>
-      </c>
-      <c r="B2" t="s">
-        <v>131</v>
       </c>
     </row>
   </sheetData>
@@ -1568,18 +1977,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A2"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <sheetData>
     <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="2" spans="1:1">
       <c r="A2" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
   </sheetData>
@@ -1591,80 +2000,80 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="15.453125" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11.6328125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.6328125" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="18.6328125" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="12.90625" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="4.54296875" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="15.453125" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="11.6328125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="19.6328125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="18.6328125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="12.90625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="4.54296875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" t="s">
+        <v>133</v>
+      </c>
+      <c r="B1" t="s">
         <v>134</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>135</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>136</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>137</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>138</v>
-      </c>
-      <c r="F1" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" t="s">
+        <v>139</v>
+      </c>
+      <c r="B2" t="s">
         <v>140</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>141</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E2" t="s">
         <v>142</v>
       </c>
-      <c r="D2" t="s">
-        <v>86</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="F2" s="3" t="s">
         <v>143</v>
-      </c>
-      <c r="F2" s="3" t="s">
-        <v>144</v>
       </c>
     </row>
     <row r="3" spans="1:6">
       <c r="C3" t="s">
+        <v>144</v>
+      </c>
+      <c r="D3" t="s">
+        <v>99</v>
+      </c>
+      <c r="E3" t="s">
         <v>145</v>
-      </c>
-      <c r="D3" t="s">
-        <v>100</v>
-      </c>
-      <c r="E3" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="4" spans="1:6">
       <c r="C4" t="s">
+        <v>146</v>
+      </c>
+      <c r="D4" t="s">
+        <v>101</v>
+      </c>
+      <c r="E4" t="s">
         <v>147</v>
-      </c>
-      <c r="D4" t="s">
-        <v>102</v>
-      </c>
-      <c r="E4" t="s">
-        <v>148</v>
       </c>
     </row>
   </sheetData>
@@ -1682,23 +2091,23 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="2" max="2" width="29.81640625" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" customWidth="true" width="29.81640625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B1" t="s">
         <v>149</v>
-      </c>
-      <c r="B1" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>151</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>152</v>
       </c>
     </row>
   </sheetData>
@@ -1716,52 +2125,52 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
   <cols>
-    <col min="1" max="1" width="22" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="10.54296875" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="14" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="22.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="10.54296875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="14.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C1" t="s">
         <v>137</v>
       </c>
-      <c r="C1" t="s">
-        <v>138</v>
-      </c>
       <c r="D1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" t="s">
+        <v>153</v>
+      </c>
+      <c r="B2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C2" t="s">
         <v>154</v>
       </c>
-      <c r="B2" t="s">
-        <v>95</v>
-      </c>
-      <c r="C2" t="s">
-        <v>155</v>
-      </c>
       <c r="D2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="D3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="D4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="D5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>